<commit_message>
Added ReportComment and DeleteComment API calls, finally.  Surrounded Http Request in Parse with Try/Catch.  Removed useless hackish _prev field of YakObject.
</commit_message>
<xml_diff>
--- a/YikYak/API Grid.xlsx
+++ b/YikYak/API Grid.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="46">
   <si>
     <t>registerUser</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>(Removed)</t>
+  </si>
+  <si>
+    <t>reportComment</t>
+  </si>
+  <si>
+    <t>deleteComment</t>
   </si>
 </sst>
 </file>
@@ -1416,10 +1422,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1460,16 +1466,16 @@
         <v>2</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>7</v>
@@ -1503,14 +1509,14 @@
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
-      <c r="F3" s="10" t="s">
-        <v>34</v>
-      </c>
+      <c r="F3" s="11"/>
       <c r="G3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="11"/>
+      <c r="H3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="10"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
@@ -1586,9 +1592,9 @@
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
+      <c r="F6" s="14"/>
       <c r="G6" s="15"/>
-      <c r="H6" s="14"/>
+      <c r="H6" s="15"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
@@ -1610,13 +1616,13 @@
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="26"/>
-      <c r="F7" s="27" t="s">
-        <v>34</v>
-      </c>
+      <c r="F7" s="26"/>
       <c r="G7" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="26"/>
+      <c r="H7" s="27" t="s">
+        <v>34</v>
+      </c>
       <c r="I7" s="26"/>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
@@ -1646,13 +1652,13 @@
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="14"/>
-      <c r="F8" s="15" t="s">
-        <v>34</v>
-      </c>
+      <c r="F8" s="14"/>
       <c r="G8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="14"/>
+      <c r="H8" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
@@ -1678,9 +1684,9 @@
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="15"/>
-      <c r="H9" s="14"/>
+      <c r="H9" s="15"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
@@ -1702,9 +1708,9 @@
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
+      <c r="F10" s="14"/>
       <c r="G10" s="15"/>
-      <c r="H10" s="14"/>
+      <c r="H10" s="15"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
@@ -1726,13 +1732,13 @@
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="15" t="s">
-        <v>34</v>
-      </c>
+      <c r="F11" s="14"/>
       <c r="G11" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="14"/>
+      <c r="H11" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
@@ -1758,13 +1764,13 @@
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="14"/>
-      <c r="F12" s="15" t="s">
-        <v>34</v>
-      </c>
+      <c r="F12" s="14"/>
       <c r="G12" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="14"/>
+      <c r="H12" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
@@ -1790,13 +1796,13 @@
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="14"/>
-      <c r="F13" s="15" t="s">
-        <v>34</v>
-      </c>
+      <c r="F13" s="14"/>
       <c r="G13" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="14"/>
+      <c r="H13" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="I13" s="14"/>
       <c r="J13" s="15"/>
       <c r="K13" s="14"/>
@@ -1870,10 +1876,10 @@
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="F16" s="15"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
-      <c r="I16" s="15"/>
+      <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
@@ -1894,10 +1900,10 @@
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+      <c r="F17" s="15"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
-      <c r="I17" s="15"/>
+      <c r="I17" s="14"/>
       <c r="J17" s="15"/>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
@@ -1918,13 +1924,13 @@
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="14"/>
-      <c r="F18" s="15" t="s">
-        <v>34</v>
-      </c>
+      <c r="F18" s="14"/>
       <c r="G18" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="14"/>
+      <c r="H18" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="I18" s="14"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
@@ -1949,79 +1955,77 @@
         <v>39</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="14"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
       <c r="I19" s="14"/>
       <c r="J19" s="15"/>
-      <c r="K19" s="14"/>
+      <c r="K19" s="15"/>
       <c r="L19" s="14"/>
       <c r="M19" s="15"/>
-      <c r="N19" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="O19" s="16" t="s">
-        <v>34</v>
-      </c>
+      <c r="N19" s="15"/>
+      <c r="O19" s="16"/>
       <c r="Q19" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="32"/>
-      <c r="B20" s="6" t="s">
-        <v>38</v>
+      <c r="B20" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="17"/>
+        <v>26</v>
+      </c>
+      <c r="D20" s="13"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
+      <c r="G20" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
+      <c r="J20" s="15"/>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
       <c r="M20" s="15"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="18"/>
-      <c r="Q20" s="5">
-        <v>1</v>
+      <c r="N20" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="O20" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="32"/>
-      <c r="B21" s="6" t="s">
-        <v>38</v>
+      <c r="B21" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
       <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
+      <c r="J21" s="15"/>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
       <c r="M21" s="15"/>
       <c r="N21" s="15"/>
       <c r="O21" s="16"/>
-      <c r="Q21" s="5">
-        <v>1</v>
-      </c>
+      <c r="Q21" s="5"/>
     </row>
     <row r="22" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="32"/>
@@ -2029,33 +2033,81 @@
         <v>38</v>
       </c>
       <c r="C22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="18"/>
+      <c r="Q22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="32"/>
+      <c r="B23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="16"/>
+      <c r="Q23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="32"/>
+      <c r="B24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="22"/>
-      <c r="Q22" s="5" t="s">
+      <c r="D24" s="19"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="22"/>
+      <c r="Q24" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:O1"/>
-    <mergeCell ref="A2:A22"/>
+    <mergeCell ref="A2:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated to match official update v2.6.1.  Not yet tested in practice, but should continue to work in theory!  Note change to HasDangerousWording.
</commit_message>
<xml_diff>
--- a/YikYak/API Grid.xlsx
+++ b/YikYak/API Grid.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
   </bookViews>
   <sheets>
-    <sheet name="2.4.2 API" sheetId="2" r:id="rId1"/>
+    <sheet name="2.6.1 API" sheetId="6" r:id="rId1"/>
     <sheet name="2.5.1 API" sheetId="4" r:id="rId2"/>
+    <sheet name="2.4.2 API" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="52">
   <si>
     <t>registerUser</t>
   </si>
@@ -163,6 +164,24 @@
   </si>
   <si>
     <t>deleteComment</t>
+  </si>
+  <si>
+    <t>bc</t>
+  </si>
+  <si>
+    <t>(0 or 1)</t>
+  </si>
+  <si>
+    <t>Omit 'bc' if Custom Peek Location</t>
+  </si>
+  <si>
+    <t>getMyTops</t>
+  </si>
+  <si>
+    <t>This would appear to perform getMyRecentReplies sorted by 'hot' order</t>
+  </si>
+  <si>
+    <t>Omit 'bc' if using to search for Custom Peek Location</t>
   </si>
 </sst>
 </file>
@@ -396,7 +415,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -481,6 +500,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -489,6 +511,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -779,6 +804,1450 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="18" width="11.7109375" customWidth="1"/>
+    <col min="20" max="20" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="32"/>
+    </row>
+    <row r="2" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="33"/>
+      <c r="B3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="33"/>
+      <c r="B4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="16"/>
+      <c r="R4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="33"/>
+      <c r="B5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="16"/>
+      <c r="R5" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="33"/>
+      <c r="B6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="16"/>
+      <c r="R6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="33"/>
+      <c r="B7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="33"/>
+      <c r="B8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="16"/>
+      <c r="R8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="33"/>
+      <c r="B9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="16"/>
+      <c r="R9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="33"/>
+      <c r="B10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="33"/>
+      <c r="B11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="33"/>
+      <c r="B12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="P12" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="33"/>
+      <c r="B13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="14"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="33"/>
+      <c r="B14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="16"/>
+      <c r="R14" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="33"/>
+      <c r="B15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="16"/>
+      <c r="R15" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="33"/>
+      <c r="B16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="16"/>
+      <c r="R16" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="33"/>
+      <c r="B17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="16"/>
+      <c r="R17" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="33"/>
+      <c r="B18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" s="14"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="P18" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="33"/>
+      <c r="B19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="16"/>
+      <c r="R19" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="33"/>
+      <c r="B20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" s="14"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="P20" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="33"/>
+      <c r="B21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="16"/>
+      <c r="R21" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="33"/>
+      <c r="B22" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="18"/>
+      <c r="R22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="33"/>
+      <c r="B23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="16"/>
+      <c r="R23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="33"/>
+      <c r="B24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="22"/>
+      <c r="R24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:P1"/>
+    <mergeCell ref="A2:A24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="17" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="32"/>
+    </row>
+    <row r="2" spans="1:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="33"/>
+      <c r="B3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="33"/>
+      <c r="B4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="16"/>
+      <c r="Q4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="33"/>
+      <c r="B5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="16"/>
+      <c r="Q5" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="33"/>
+      <c r="B6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="16"/>
+      <c r="Q6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="33"/>
+      <c r="B7" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="33"/>
+      <c r="B8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="33"/>
+      <c r="B9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="16"/>
+      <c r="Q9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="33"/>
+      <c r="B10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="16"/>
+      <c r="Q10" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="33"/>
+      <c r="B11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="O11" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="33"/>
+      <c r="B12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="O12" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="33"/>
+      <c r="B13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="O13" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="33"/>
+      <c r="B14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="16"/>
+      <c r="Q14" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="33"/>
+      <c r="B15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="16"/>
+      <c r="Q15" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="33"/>
+      <c r="B16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="16"/>
+      <c r="Q16" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="33"/>
+      <c r="B17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="16"/>
+      <c r="Q17" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="33"/>
+      <c r="B18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="O18" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="33"/>
+      <c r="B19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="16"/>
+      <c r="Q19" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="33"/>
+      <c r="B20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="14"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="O20" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="33"/>
+      <c r="B21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="16"/>
+      <c r="Q21" s="5"/>
+    </row>
+    <row r="22" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="33"/>
+      <c r="B22" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="18"/>
+      <c r="Q22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="33"/>
+      <c r="B23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="16"/>
+      <c r="Q23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="33"/>
+      <c r="B24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="19"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="22"/>
+      <c r="Q24" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="A2:A24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -793,24 +2262,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="32"/>
     </row>
     <row r="2" spans="1:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="3"/>
@@ -856,7 +2325,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
+      <c r="A3" s="33"/>
       <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
@@ -888,7 +2357,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="6" t="s">
         <v>38</v>
       </c>
@@ -912,7 +2381,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="5" t="s">
         <v>39</v>
       </c>
@@ -939,7 +2408,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="5" t="s">
         <v>39</v>
       </c>
@@ -963,7 +2432,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
@@ -995,7 +2464,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="5" t="s">
         <v>39</v>
       </c>
@@ -1027,7 +2496,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="5" t="s">
         <v>39</v>
       </c>
@@ -1051,7 +2520,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="5" t="s">
         <v>39</v>
       </c>
@@ -1075,7 +2544,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="5" t="s">
         <v>39</v>
       </c>
@@ -1107,7 +2576,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="5" t="s">
         <v>39</v>
       </c>
@@ -1139,7 +2608,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="5" t="s">
         <v>39</v>
       </c>
@@ -1171,7 +2640,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="5" t="s">
         <v>39</v>
       </c>
@@ -1195,7 +2664,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="5" t="s">
         <v>39</v>
       </c>
@@ -1219,7 +2688,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="5" t="s">
         <v>39</v>
       </c>
@@ -1243,7 +2712,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
+      <c r="A17" s="33"/>
       <c r="B17" s="5" t="s">
         <v>39</v>
       </c>
@@ -1267,7 +2736,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
+      <c r="A18" s="33"/>
       <c r="B18" s="5" t="s">
         <v>39</v>
       </c>
@@ -1302,7 +2771,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="32"/>
+      <c r="A19" s="33"/>
       <c r="B19" s="5" t="s">
         <v>39</v>
       </c>
@@ -1334,7 +2803,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="32"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="6" t="s">
         <v>38</v>
       </c>
@@ -1358,7 +2827,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="32"/>
+      <c r="A21" s="33"/>
       <c r="B21" s="6" t="s">
         <v>38</v>
       </c>
@@ -1382,7 +2851,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="32"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="6" t="s">
         <v>38</v>
       </c>
@@ -1418,698 +2887,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="17" width="11.7109375" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="31"/>
-    </row>
-    <row r="2" spans="1:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
-      <c r="B3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32"/>
-      <c r="B4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="16"/>
-      <c r="Q4" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
-      <c r="B5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="16"/>
-      <c r="Q5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="S5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
-      <c r="B6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="16"/>
-      <c r="Q6" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="O7" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="S7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
-      <c r="B8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="O8" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="16"/>
-      <c r="Q9" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
-      <c r="B10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="16"/>
-      <c r="Q10" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
-      <c r="B11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="O11" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="O12" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q12" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="O13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q13" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="16"/>
-      <c r="Q14" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
-      <c r="B15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="16"/>
-      <c r="Q15" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
-      <c r="B16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="16"/>
-      <c r="Q16" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
-      <c r="B17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="16"/>
-      <c r="Q17" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
-      <c r="B18" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="O18" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="S18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="32"/>
-      <c r="B19" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="16"/>
-      <c r="Q19" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="32"/>
-      <c r="B20" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I20" s="14"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="O20" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q20" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="32"/>
-      <c r="B21" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="16"/>
-      <c r="Q21" s="5"/>
-    </row>
-    <row r="22" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="32"/>
-      <c r="B22" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="18"/>
-      <c r="Q22" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="32"/>
-      <c r="B23" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="16"/>
-      <c r="Q23" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="32"/>
-      <c r="B24" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="22"/>
-      <c r="Q24" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="A2:A24"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>